<commit_message>
add new data after changing the way to random principal point
</commit_message>
<xml_diff>
--- a/data_synthetic/AIC_resuls.xlsx
+++ b/data_synthetic/AIC_resuls.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="161">
   <si>
     <t>ind</t>
   </si>
@@ -40,7 +40,7 @@
     <t>data_synthetic/synthetic_img_pt1.npy</t>
   </si>
   <si>
-    <t>[580.   0. 640.   0. 580. 480.   0.   0.   1.]</t>
+    <t>[605.   0. 640.   0. 605. 480.   0.   0.   1.]</t>
   </si>
   <si>
     <t>[0. 0. 0. 0. 0.]</t>
@@ -52,10 +52,10 @@
     <t>data_synthetic/synthetic_img_pt2.npy</t>
   </si>
   <si>
-    <t>[558.   0. 640.   0. 558. 480.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.08 0.   0.   0.   0.  ]</t>
+    <t>[813.   0. 640.   0. 813. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.03 0.   0.   0.   0.  ]</t>
   </si>
   <si>
     <t>{'type': 'normal', 'f': 'f', 'dist': 'k1'}</t>
@@ -67,22 +67,25 @@
     <t>data_synthetic/synthetic_img_pt3.npy</t>
   </si>
   <si>
-    <t>[631.   0. 640.   0. 631. 480.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.05 0.06 0.   0.   0.  ]</t>
+    <t>[803.   0. 640.   0. 803. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.05 0.01 0.   0.   0.  ]</t>
   </si>
   <si>
     <t>{'type': 'normal', 'f': 'f', 'dist': 'k1_k2'}</t>
   </si>
   <si>
+    <t>{'type': 'normal', 'f': 'fx_fy', 'dist': 'k1_k2'}</t>
+  </si>
+  <si>
     <t>data_synthetic/synthetic_img_pt4.npy</t>
   </si>
   <si>
-    <t>[734.   0. 640.   0. 734. 480.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.01 0.02 0.05 0.   0.  ]</t>
+    <t>[650.   0. 640.   0. 650. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.07 0.04 0.05 0.   0.  ]</t>
   </si>
   <si>
     <t>{'type': 'normal', 'f': 'f', 'dist': 'k1_k2_k3'}</t>
@@ -94,16 +97,16 @@
     <t>data_synthetic/synthetic_img_pt5.npy</t>
   </si>
   <si>
-    <t>[617.   0. 640.   0. 617. 480.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.01 0.01 0.02 0.05 0.02]</t>
+    <t>[783.   0. 640.   0. 783. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.06 0.02 0.05 0.07 0.02]</t>
   </si>
   <si>
     <t>data_synthetic/synthetic_img_pt6.npy</t>
   </si>
   <si>
-    <t>[914.   0. 640.   0. 842. 480.   0.   0.   1.]</t>
+    <t>[654.   0. 640.   0. 556. 480.   0.   0.   1.]</t>
   </si>
   <si>
     <t>{'type': 'normal', 'f': 'fx_fy', 'dist': 'no'}</t>
@@ -112,160 +115,402 @@
     <t>data_synthetic/synthetic_img_pt7.npy</t>
   </si>
   <si>
-    <t>[912.   0. 640.   0. 842. 480.   0.   0.   1.]</t>
+    <t>[559.   0. 640.   0. 997. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.02 0.   0.   0.   0.  ]</t>
   </si>
   <si>
     <t>data_synthetic/synthetic_img_pt8.npy</t>
   </si>
   <si>
-    <t>[954.   0. 640.   0. 926. 480.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.09 0.03 0.   0.   0.  ]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'fx_fy', 'dist': 'k1_k2'}</t>
+    <t>[766.   0. 640.   0. 809. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.06 0.07 0.   0.   0.  ]</t>
   </si>
   <si>
     <t>data_synthetic/synthetic_img_pt9.npy</t>
   </si>
   <si>
-    <t>[708.   0. 640.   0. 667. 480.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.05 0.04 0.02 0.   0.  ]</t>
+    <t>[993.   0. 640.   0. 929. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.07 0.01 0.07 0.   0.  ]</t>
   </si>
   <si>
     <t>{'type': 'normal', 'f': 'fx_fy', 'dist': 'k1_k2_k3'}</t>
   </si>
   <si>
+    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'k1_k2_p1_p2_k3'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt10.npy</t>
+  </si>
+  <si>
+    <t>[529.   0. 640.   0. 920. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.01 0.01 0.04 0.02 0.04]</t>
+  </si>
+  <si>
     <t>{'type': 'normal', 'f': 'fx_fy', 'dist': 'k1_k2_p1_p2_k3'}</t>
   </si>
   <si>
-    <t>data_synthetic/synthetic_img_pt10.npy</t>
-  </si>
-  <si>
-    <t>[634.   0. 640.   0. 869. 480.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.01 0.   0.07 0.03 0.01]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'k1_k2_p1_p2_k3'}</t>
+    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2_p1_p2_k3'}</t>
   </si>
   <si>
     <t>data_synthetic/synthetic_img_pt11.npy</t>
   </si>
   <si>
-    <t>[7.260e+02 0.000e+00 1.193e+03 0.000e+00 7.260e+02 7.890e+02 0.000e+00
+    <t>[902.   0. 838.   0. 902. 957.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'no'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt12.npy</t>
+  </si>
+  <si>
+    <t>[725.   0. 784.   0. 725. 807.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.05 0.   0.   0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'k1'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt13.npy</t>
+  </si>
+  <si>
+    <t>[748.   0. 882.   0. 748. 730.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.09 0.05 0.   0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'k1_k2'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt14.npy</t>
+  </si>
+  <si>
+    <t>[948.   0. 753.   0. 948.  90.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.05 0.08 0.06 0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'k1_k2_k3'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt15.npy</t>
+  </si>
+  <si>
+    <t>[551.   0. 637.   0. 551. 636.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.07 0.08 0.01 0.08 0.05]</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt16.npy</t>
+  </si>
+  <si>
+    <t>[918.   0. 985.   0. 981. 317.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'no'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt17.npy</t>
+  </si>
+  <si>
+    <t>[952.   0. 209.   0. 552. 604.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'k1'}</t>
+  </si>
+  <si>
+    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt18.npy</t>
+  </si>
+  <si>
+    <t>[676.   0. 479.   0. 675. 659.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.06 0.01 0.   0.   0.  ]</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt19.npy</t>
+  </si>
+  <si>
+    <t>[676.   0. 759.   0. 973. 324.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.02 0.07 0.02 0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2_k3'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt20.npy</t>
+  </si>
+  <si>
+    <t>[5.990e+02 0.000e+00 1.032e+03 0.000e+00 6.420e+02 4.950e+02 0.000e+00
  0.000e+00 1.000e+00]</t>
   </si>
   <si>
-    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'no'}</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt12.npy</t>
-  </si>
-  <si>
-    <t>[761.   0. 919.   0. 761. 264.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.09 0.   0.   0.   0.  ]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'k1'}</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt13.npy</t>
-  </si>
-  <si>
-    <t>[8.570e+02 0.000e+00 1.037e+03 0.000e+00 8.570e+02 9.010e+02 0.000e+00
+    <t>[0.07 0.06 0.07 0.02 0.06]</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt21.npy</t>
+  </si>
+  <si>
+    <t>[858.   0. 640.   0. 540. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0. 0. 0. 0.]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy', 'dist': 'no'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt22.npy</t>
+  </si>
+  <si>
+    <t>[865.   0. 640.   0. 607. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.06 0.   0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy', 'dist': 'k1'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt23.npy</t>
+  </si>
+  <si>
+    <t>[743.   0. 640.   0. 610. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.08 0.01 0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy', 'dist': 'k1_k2'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt24.npy</t>
+  </si>
+  <si>
+    <t>[756.   0. 640.   0. 570. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.07 0.08 0.05 0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy', 'dist': 'k1_k2_k3'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt25.npy</t>
+  </si>
+  <si>
+    <t>[915.   0. 640.   0. 625. 480.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.02 0.02 0.03 0.03]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy', 'dist': 'k1_k2_k3_k4'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt26.npy</t>
+  </si>
+  <si>
+    <t>[6.64e+02 9.00e-02 6.40e+02 0.00e+00 7.58e+02 4.80e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_s', 'dist': 'no'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt27.npy</t>
+  </si>
+  <si>
+    <t>[8.63e+02 2.00e-02 6.40e+02 0.00e+00 8.43e+02 4.80e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>[0.04 0.   0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_s', 'dist': 'k1'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt28.npy</t>
+  </si>
+  <si>
+    <t>[6.61e+02 1.00e-02 6.40e+02 0.00e+00 7.87e+02 4.80e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>[0.   0.07 0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_s', 'dist': 'k1_k2'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt29.npy</t>
+  </si>
+  <si>
+    <t>[8.31e+02 2.00e-02 6.40e+02 0.00e+00 5.10e+02 4.80e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>[0.06 0.08 0.04 0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_s', 'dist': 'k1_k2_k3'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt30.npy</t>
+  </si>
+  <si>
+    <t>[8.23e+02 4.00e-02 6.40e+02 0.00e+00 9.25e+02 4.80e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>[0.   0.06 0.02 0.05]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_s', 'dist': 'k1_k2_k3_k4'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt31.npy</t>
+  </si>
+  <si>
+    <t>[8.730e+02 0.000e+00 1.008e+03 0.000e+00 8.770e+02 7.760e+02 0.000e+00
  0.000e+00 1.000e+00]</t>
   </si>
   <si>
-    <t>[0.03 0.08 0.   0.   0.  ]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'k1_k2'}</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt14.npy</t>
-  </si>
-  <si>
-    <t>[981.   0. 392.   0. 981. 929.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.01 0.08 0.07 0.   0.  ]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'f_cx_cy', 'dist': 'k1_k2_k3'}</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2_p1_p2_k3'}</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt15.npy</t>
-  </si>
-  <si>
-    <t>[776.   0. 864.   0. 776.  10.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.06 0.02 0.03 0.08 0.04]</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt16.npy</t>
-  </si>
-  <si>
-    <t>[753.   0. 185.   0. 682. 898.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'no'}</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt17.npy</t>
-  </si>
-  <si>
-    <t>[759.   0. 240.   0. 639. 507.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.03 0.   0.   0.   0.  ]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'k1'}</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt18.npy</t>
-  </si>
-  <si>
-    <t>[918.   0. 652.   0. 705.  46.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.05 0.03 0.   0.   0.  ]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2'}</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt19.npy</t>
-  </si>
-  <si>
-    <t>[8.460e+02 0.000e+00 1.068e+03 0.000e+00 9.250e+02 8.080e+02 0.000e+00
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy', 'dist': 'no'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt32.npy</t>
+  </si>
+  <si>
+    <t>[9.960e+02 0.000e+00 1.201e+03 0.000e+00 8.970e+02 1.590e+02 0.000e+00
  0.000e+00 1.000e+00]</t>
   </si>
   <si>
-    <t>[0.03 0.03 0.07 0.   0.  ]</t>
-  </si>
-  <si>
-    <t>{'type': 'normal', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2_k3'}</t>
-  </si>
-  <si>
-    <t>data_synthetic/synthetic_img_pt20.npy</t>
-  </si>
-  <si>
-    <t>[994.   0. 353.   0. 948. 572.   0.   0.   1.]</t>
-  </si>
-  <si>
-    <t>[0.04 0.07 0.02 0.07 0.01]</t>
+    <t>[0.08 0.   0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy', 'dist': 'k1'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt33.npy</t>
+  </si>
+  <si>
+    <t>[8.790e+02 0.000e+00 1.194e+03 0.000e+00 8.040e+02 5.290e+02 0.000e+00
+ 0.000e+00 1.000e+00]</t>
+  </si>
+  <si>
+    <t>[0.   0.09 0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt34.npy</t>
+  </si>
+  <si>
+    <t>[698.   0. 547.   0. 529. 605.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.08 0.06 0.04 0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2_k3'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt35.npy</t>
+  </si>
+  <si>
+    <t>[869.   0. 303.   0. 510. 871.   0.   0.   1.]</t>
+  </si>
+  <si>
+    <t>[0.07 0.01 0.05 0.02]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy', 'dist': 'k1_k2_k3_k4'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt36.npy</t>
+  </si>
+  <si>
+    <t>[6.29e+02 8.00e-02 4.03e+02 0.00e+00 7.83e+02 2.42e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy_s', 'dist': 'no'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt37.npy</t>
+  </si>
+  <si>
+    <t>[9.300e+02 1.000e-02 1.197e+03 0.000e+00 8.910e+02 4.940e+02 0.000e+00
+ 0.000e+00 1.000e+00]</t>
+  </si>
+  <si>
+    <t>[0.01 0.   0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy_s', 'dist': 'k1'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt38.npy</t>
+  </si>
+  <si>
+    <t>[5.39e+02 3.00e-02 5.12e+02 0.00e+00 7.66e+02 3.85e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>[0.09 0.02 0.   0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy_s', 'dist': 'k1_k2'}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt39.npy</t>
+  </si>
+  <si>
+    <t>[6.71e+02 3.00e-02 1.03e+03 0.00e+00 9.02e+02 2.27e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>[0.02 0.01 0.08 0.  ]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy_s', 'dist': 'k1_k2_k3'}</t>
+  </si>
+  <si>
+    <t>{'type': '', 'f': '', 'dist': ''}</t>
+  </si>
+  <si>
+    <t>data_synthetic/synthetic_img_pt40.npy</t>
+  </si>
+  <si>
+    <t>[6.51e+02 6.00e-02 8.67e+02 0.00e+00 7.41e+02 9.59e+02 0.00e+00 0.00e+00
+ 1.00e+00]</t>
+  </si>
+  <si>
+    <t>[0.07 0.08 0.02 0.04]</t>
+  </si>
+  <si>
+    <t>{'type': 'fisheye', 'f': 'fx_fy_cx_cy_s', 'dist': 'k1_k2_k3_k4'}</t>
   </si>
 </sst>
 </file>
@@ -673,17 +918,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
     <col min="6" max="6" style="10" width="47.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="10" width="47.43357142857143" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -736,7 +981,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="7">
-        <v>4.437271177768707</v>
+        <v>5.652013838291168</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -762,7 +1007,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="7">
-        <v>7.503415405750275</v>
+        <v>7.65596604347229</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -785,10 +1030,10 @@
         <v>19</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4" s="7">
-        <v>6.620260834693909</v>
+        <v>10.04332172870636</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -799,22 +1044,22 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" s="7">
-        <v>13.20628625154495</v>
+        <v>14.25473195314407</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -825,22 +1070,22 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H6" s="7">
-        <v>12.53424388170242</v>
+        <v>12.41816383600235</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -851,22 +1096,22 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" s="7">
-        <v>4.31299889087677</v>
+        <v>5.300051808357239</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -877,22 +1122,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H8" s="7">
-        <v>7.451406955718994</v>
+        <v>6.303424894809723</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -903,22 +1148,22 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H9" s="7">
-        <v>9.279599964618683</v>
+        <v>8.02209097146988</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -929,22 +1174,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H10" s="7">
-        <v>14.37346035242081</v>
+        <v>802.2812280654907</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -955,25 +1200,25 @@
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H11" s="7">
-        <v>4464.622055351734</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="32.25">
+        <v>19.92172825336456</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -981,22 +1226,22 @@
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H12" s="7">
-        <v>6.347417175769806</v>
+        <v>7.296587288379669</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1007,25 +1252,25 @@
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H13" s="7">
-        <v>9.791724935173988</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="32.25">
+        <v>8.276565551757812</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1033,22 +1278,22 @@
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="H14" s="7">
-        <v>1685.535074710846</v>
+        <v>10.11026859283447</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -1059,22 +1304,22 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="H15" s="7">
-        <v>28028.05062647164</v>
+        <v>2524.701386395842</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -1085,22 +1330,22 @@
         <v>15</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H16" s="7">
-        <v>2053.254509195918</v>
+        <v>18.78688967227936</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -1111,25 +1356,25 @@
         <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="H17" s="7">
-        <v>7.229830086231232</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+        <v>5.569390296936035</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1137,25 +1382,25 @@
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="H18" s="7">
-        <v>278.4134922027588</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+        <v>929.8309910930693</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1163,22 +1408,22 @@
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="G19" s="6" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="H19" s="7">
-        <v>68.1685993084684</v>
+        <v>10.56573189795017</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
@@ -1201,10 +1446,10 @@
         <v>79</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H20" s="7">
-        <v>232.9341221451759</v>
+        <v>172.3403510004282</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
@@ -1224,13 +1469,533 @@
         <v>82</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="H21" s="7">
-        <v>36.99977214634418</v>
+        <v>9679.190320134163</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="7">
+        <v>2188.738933384418</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="7">
+        <v>7787.36567980051</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="7">
+        <v>14.8440762758255</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="7">
+        <v>10.38895756006241</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="7">
+        <v>2786.246876835823</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5">
+        <v>26</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="7">
+        <v>11587.12023025751</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="2">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5">
+        <v>27</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="7">
+        <v>85.94560360908508</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="2">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5">
+        <v>28</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="7">
+        <v>7495.313852369785</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="2">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H30" s="7">
+        <v>15.71597367525101</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="2">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5">
+        <v>30</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="7">
+        <v>10999.70371210575</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="5">
+        <v>31</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="7">
+        <v>812.4927669167519</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="A33" s="2">
+        <v>31</v>
+      </c>
+      <c r="B33" s="5">
+        <v>32</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" s="7">
+        <v>1552.200164213777</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="A34" s="2">
+        <v>32</v>
+      </c>
+      <c r="B34" s="5">
+        <v>33</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="7">
+        <v>3864.477937281132</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="A35" s="2">
+        <v>33</v>
+      </c>
+      <c r="B35" s="5">
+        <v>34</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H35" s="7">
+        <v>14.69946981966496</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="A36" s="2">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5">
+        <v>35</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="7">
+        <v>556.1068646460772</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="5">
+        <v>36</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="7">
+        <v>3068.188772708178</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="A38" s="2">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <v>37</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" s="7">
+        <v>5332.535109102726</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+      <c r="A39" s="2">
+        <v>37</v>
+      </c>
+      <c r="B39" s="5">
+        <v>38</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" s="7">
+        <v>14.22579915821552</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+      <c r="A40" s="2">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5">
+        <v>39</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H40" s="5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="2">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5">
+        <v>40</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="7">
+        <v>3526.9766741395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>